<commit_message>
More tested, adjusted temnplate slightly
</commit_message>
<xml_diff>
--- a/adapterFPix2DTBTestProtocol_template.xlsx
+++ b/adapterFPix2DTBTestProtocol_template.xlsx
@@ -575,9 +575,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -605,6 +602,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="155">
@@ -1107,8 +1107,8 @@
   </sheetPr>
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1133,7 +1133,7 @@
       <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="18" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1190,10 +1190,10 @@
       <c r="G11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>57</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -1202,7 +1202,7 @@
       <c r="L11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O11" s="23" t="s">
+      <c r="O11" s="22" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1233,12 +1233,13 @@
       <c r="J12" t="s">
         <v>14</v>
       </c>
+      <c r="K12" s="12"/>
       <c r="L12" s="9" t="str">
-        <f>IF(K12&lt;K$28,"ok","NOK")</f>
+        <f t="shared" ref="L12:L27" si="0">IF(K12&lt;K$28,"ok","NOK")</f>
         <v>ok</v>
       </c>
       <c r="O12">
-        <f>IF(G12="NOK",1,0)</f>
+        <f t="shared" ref="O12:O45" si="1">IF(G12="NOK",1,0)</f>
         <v>1</v>
       </c>
       <c r="P12">
@@ -1273,16 +1274,17 @@
       <c r="J13" t="s">
         <v>15</v>
       </c>
+      <c r="K13" s="12"/>
       <c r="L13" s="9" t="str">
-        <f>IF(K13&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O13">
-        <f>IF(G13="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:P27" si="0">IF(L13="NOK",1,0)</f>
+        <f t="shared" ref="P13:P27" si="2">IF(L13="NOK",1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1314,16 +1316,17 @@
       <c r="J14" t="s">
         <v>10</v>
       </c>
+      <c r="K14" s="12"/>
       <c r="L14" s="9" t="str">
-        <f>IF(K14&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O14">
-        <f>IF(G14="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1355,16 +1358,17 @@
       <c r="J15" t="s">
         <v>10</v>
       </c>
+      <c r="K15" s="12"/>
       <c r="L15" s="9" t="str">
-        <f>IF(K15&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O15">
-        <f>IF(G15="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1395,16 +1399,17 @@
       <c r="J16" t="s">
         <v>16</v>
       </c>
+      <c r="K16" s="12"/>
       <c r="L16" s="9" t="str">
-        <f>IF(K16&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O16">
-        <f>IF(G16="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1435,16 +1440,17 @@
       <c r="J17" t="s">
         <v>17</v>
       </c>
+      <c r="K17" s="12"/>
       <c r="L17" s="9" t="str">
-        <f>IF(K17&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O17">
-        <f>IF(G17="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1475,16 +1481,17 @@
       <c r="J18" t="s">
         <v>18</v>
       </c>
+      <c r="K18" s="12"/>
       <c r="L18" s="9" t="str">
-        <f>IF(K18&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O18">
-        <f>IF(G18="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1515,16 +1522,17 @@
       <c r="J19" t="s">
         <v>19</v>
       </c>
+      <c r="K19" s="12"/>
       <c r="L19" s="9" t="str">
-        <f>IF(K19&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O19">
-        <f>IF(G19="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1546,7 +1554,7 @@
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="5" t="str">
-        <f t="shared" ref="G20:G25" si="1">IF(F20="∞","ok","NOK")</f>
+        <f t="shared" ref="G20:G25" si="3">IF(F20="∞","ok","NOK")</f>
         <v>NOK</v>
       </c>
       <c r="I20">
@@ -1555,16 +1563,17 @@
       <c r="J20" t="s">
         <v>20</v>
       </c>
+      <c r="K20" s="12"/>
       <c r="L20" s="9" t="str">
-        <f>IF(K20&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O20">
-        <f>IF(G20="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1586,7 +1595,7 @@
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>NOK</v>
       </c>
       <c r="I21">
@@ -1595,16 +1604,17 @@
       <c r="J21" t="s">
         <v>21</v>
       </c>
+      <c r="K21" s="12"/>
       <c r="L21" s="9" t="str">
-        <f>IF(K21&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O21">
-        <f>IF(G21="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1626,7 +1636,7 @@
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>NOK</v>
       </c>
       <c r="I22">
@@ -1635,16 +1645,17 @@
       <c r="J22" t="s">
         <v>22</v>
       </c>
+      <c r="K22" s="12"/>
       <c r="L22" s="9" t="str">
-        <f>IF(K22&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O22">
-        <f>IF(G22="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1666,7 +1677,7 @@
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>NOK</v>
       </c>
       <c r="I23">
@@ -1675,16 +1686,17 @@
       <c r="J23" t="s">
         <v>23</v>
       </c>
+      <c r="K23" s="12"/>
       <c r="L23" s="9" t="str">
-        <f>IF(K23&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O23">
-        <f>IF(G23="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1706,7 +1718,7 @@
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>NOK</v>
       </c>
       <c r="I24">
@@ -1715,16 +1727,17 @@
       <c r="J24" t="s">
         <v>11</v>
       </c>
+      <c r="K24" s="12"/>
       <c r="L24" s="9" t="str">
-        <f>IF(K24&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O24">
-        <f>IF(G24="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1746,7 +1759,7 @@
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>NOK</v>
       </c>
       <c r="I25">
@@ -1755,16 +1768,17 @@
       <c r="J25" t="s">
         <v>11</v>
       </c>
+      <c r="K25" s="12"/>
       <c r="L25" s="9" t="str">
-        <f>IF(K25&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O25">
-        <f>IF(G25="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1796,16 +1810,17 @@
       <c r="J26" t="s">
         <v>12</v>
       </c>
+      <c r="K26" s="12"/>
       <c r="L26" s="9" t="str">
-        <f>IF(K26&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O26">
-        <f>IF(G26="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1836,16 +1851,17 @@
       <c r="J27" t="s">
         <v>13</v>
       </c>
+      <c r="K27" s="12"/>
       <c r="L27" s="9" t="str">
-        <f>IF(K27&lt;K$28,"ok","NOK")</f>
+        <f t="shared" si="0"/>
         <v>ok</v>
       </c>
       <c r="O27">
-        <f>IF(G27="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1874,11 +1890,11 @@
       <c r="I28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K28" s="19">
         <v>1</v>
       </c>
       <c r="O28">
-        <f>IF(G28="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1906,7 +1922,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29">
-        <f>IF(G29="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1932,16 +1948,16 @@
         <f>IF(ABS(F30-D30)&lt;=E30,"ok","NOK")</f>
         <v>NOK</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
       <c r="O30">
-        <f>IF(G30="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1966,13 +1982,13 @@
         <f>IF(F31="∞","ok","NOK")</f>
         <v>NOK</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
       <c r="O31">
-        <f>IF(G31="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1999,7 +2015,7 @@
         <v>NOK</v>
       </c>
       <c r="O32">
-        <f>IF(G32="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2024,10 +2040,10 @@
         <f>IF(F33="∞","ok","NOK")</f>
         <v>NOK</v>
       </c>
-      <c r="I33" s="21" t="s">
+      <c r="I33" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="J33" s="20" t="s">
         <v>57</v>
       </c>
       <c r="K33" s="6" t="s">
@@ -2037,7 +2053,7 @@
         <v>8</v>
       </c>
       <c r="O33">
-        <f>IF(G33="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2060,7 +2076,7 @@
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="5" t="str">
-        <f t="shared" ref="G34:G40" si="2">IF(ABS(F34-D34)&lt;=E34,"ok","NOK")</f>
+        <f t="shared" ref="G34:G40" si="4">IF(ABS(F34-D34)&lt;=E34,"ok","NOK")</f>
         <v>NOK</v>
       </c>
       <c r="I34">
@@ -2069,16 +2085,17 @@
       <c r="J34" t="s">
         <v>9</v>
       </c>
+      <c r="K34" s="12"/>
       <c r="L34" s="9" t="str">
         <f>IF(K34&lt;K$42,"ok","NOK")</f>
         <v>ok</v>
       </c>
       <c r="O34">
-        <f>IF(G34="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P34">
-        <f t="shared" ref="P34:P41" si="3">IF(L34="NOK",1,0)</f>
+        <f t="shared" ref="P34:P41" si="5">IF(L34="NOK",1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2101,7 +2118,7 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NOK</v>
       </c>
       <c r="I35">
@@ -2110,16 +2127,17 @@
       <c r="J35" t="s">
         <v>9</v>
       </c>
+      <c r="K35" s="12"/>
       <c r="L35" s="9" t="str">
-        <f t="shared" ref="L35:L41" si="4">IF(K35&lt;K$42,"ok","NOK")</f>
+        <f t="shared" ref="L35:L41" si="6">IF(K35&lt;K$42,"ok","NOK")</f>
         <v>ok</v>
       </c>
       <c r="O35">
-        <f>IF(G35="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2142,7 +2160,7 @@
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NOK</v>
       </c>
       <c r="I36">
@@ -2151,16 +2169,17 @@
       <c r="J36" t="s">
         <v>10</v>
       </c>
+      <c r="K36" s="12"/>
       <c r="L36" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="O36">
-        <f>IF(G36="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2184,7 +2203,7 @@
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NOK</v>
       </c>
       <c r="I37">
@@ -2193,16 +2212,17 @@
       <c r="J37" t="s">
         <v>9</v>
       </c>
+      <c r="K37" s="12"/>
       <c r="L37" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="O37">
-        <f>IF(G37="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2226,7 +2246,7 @@
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NOK</v>
       </c>
       <c r="I38">
@@ -2235,16 +2255,17 @@
       <c r="J38" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="K38" s="12"/>
       <c r="L38" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="O38">
-        <f>IF(G38="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2268,7 +2289,7 @@
       </c>
       <c r="F39" s="16"/>
       <c r="G39" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NOK</v>
       </c>
       <c r="I39">
@@ -2277,16 +2298,17 @@
       <c r="J39" t="s">
         <v>11</v>
       </c>
+      <c r="K39" s="12"/>
       <c r="L39" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="O39">
-        <f>IF(G39="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2309,7 +2331,7 @@
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>NOK</v>
       </c>
       <c r="I40">
@@ -2318,16 +2340,17 @@
       <c r="J40" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="K40" s="12"/>
       <c r="L40" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="O40">
-        <f>IF(G40="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2358,16 +2381,17 @@
       <c r="J41" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="K41" s="12"/>
       <c r="L41" s="9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="O41">
-        <f>IF(G41="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2399,7 +2423,7 @@
         <v>0.5</v>
       </c>
       <c r="O42">
-        <f>IF(G42="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2425,7 +2449,7 @@
         <v>NOK</v>
       </c>
       <c r="O43">
-        <f>IF(G43="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2450,14 +2474,14 @@
         <f>IF(F44="∞","ok","NOK")</f>
         <v>NOK</v>
       </c>
-      <c r="I44" s="22" t="s">
+      <c r="I44" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
       <c r="O44">
-        <f>IF(G44="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2482,14 +2506,14 @@
         <f>IF(F45="∞","ok","NOK")</f>
         <v>NOK</v>
       </c>
-      <c r="I45" s="22" t="s">
+      <c r="I45" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
       <c r="O45">
-        <f>IF(G45="NOK",1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2527,7 +2551,7 @@
       <c r="A54" t="s">
         <v>40</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2571,7 +2595,7 @@
       <c r="B64" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="29"/>
+      <c r="C64" s="28"/>
       <c r="D64" s="4" t="s">
         <v>46</v>
       </c>
@@ -2580,7 +2604,7 @@
       <c r="B65" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="29"/>
+      <c r="C65" s="28"/>
       <c r="D65" s="4" t="s">
         <v>46</v>
       </c>
@@ -2589,7 +2613,7 @@
       <c r="B66" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="26">
+      <c r="C66" s="25">
         <f>C65-C64</f>
         <v>0</v>
       </c>
@@ -2602,14 +2626,14 @@
       <c r="F66" s="5">
         <v>0.01</v>
       </c>
-      <c r="G66" s="27" t="s">
+      <c r="G66" s="26" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="C67" s="26"/>
+      <c r="C67" s="25"/>
       <c r="D67" s="4"/>
-      <c r="G67" s="27"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
@@ -2663,7 +2687,7 @@
         <v>69</v>
       </c>
       <c r="B77" s="14"/>
-      <c r="C77" s="24" t="str">
+      <c r="C77" s="23" t="str">
         <f>IF(AND(B47="PASS",B54="PASS",B68="PASS",D72="y",D73="y",D74="y"),"ACCEPTED","REJECTED")</f>
         <v>REJECTED</v>
       </c>

</xml_diff>